<commit_message>
appium word doc + test cases updations
</commit_message>
<xml_diff>
--- a/AndroidAppiumTestCases.xlsx
+++ b/AndroidAppiumTestCases.xlsx
@@ -4,24 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="682" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="682"/>
   </bookViews>
   <sheets>
-    <sheet name="HomePage" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginPage" sheetId="2" r:id="rId2"/>
-    <sheet name="CategoryListPage" sheetId="3" r:id="rId3"/>
-    <sheet name="CategoryPage" sheetId="4" r:id="rId4"/>
-    <sheet name="CartPage" sheetId="5" r:id="rId5"/>
-    <sheet name="CheckoutPage" sheetId="6" r:id="rId6"/>
-    <sheet name="ThankYouPage" sheetId="7" r:id="rId7"/>
-    <sheet name="Sprint1" sheetId="8" r:id="rId8"/>
+    <sheet name="Sprint1" sheetId="8" r:id="rId1"/>
+    <sheet name="HomePage" sheetId="1" r:id="rId2"/>
+    <sheet name="LoginPage" sheetId="2" r:id="rId3"/>
+    <sheet name="CategoryListPage" sheetId="3" r:id="rId4"/>
+    <sheet name="CategoryPage" sheetId="4" r:id="rId5"/>
+    <sheet name="CartPage" sheetId="5" r:id="rId6"/>
+    <sheet name="CheckoutPage" sheetId="6" r:id="rId7"/>
+    <sheet name="ThankYouPage" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="97">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -242,9 +242,6 @@
     <t>SignUp</t>
   </si>
   <si>
-    <t xml:space="preserve">To make user register </t>
-  </si>
-  <si>
     <t>headerVisible()</t>
   </si>
   <si>
@@ -254,9 +251,6 @@
     <t xml:space="preserve">loginGooglePlus() </t>
   </si>
   <si>
-    <t>userRegister()</t>
-  </si>
-  <si>
     <t>loginFacebook()</t>
   </si>
   <si>
@@ -276,6 +270,48 @@
   </si>
   <si>
     <t>ThankYouPage</t>
+  </si>
+  <si>
+    <t>Sections</t>
+  </si>
+  <si>
+    <t>Hot Deals</t>
+  </si>
+  <si>
+    <t>More Link</t>
+  </si>
+  <si>
+    <t>About Us</t>
+  </si>
+  <si>
+    <t>userSignUp()</t>
+  </si>
+  <si>
+    <t>To make user signup</t>
+  </si>
+  <si>
+    <t>Avtar icon</t>
+  </si>
+  <si>
+    <t>Login or Signup link</t>
+  </si>
+  <si>
+    <t>CATEGORIES</t>
+  </si>
+  <si>
+    <t>Categories list</t>
+  </si>
+  <si>
+    <t>Navigate to CategoryList page</t>
+  </si>
+  <si>
+    <t>To check hot deals present, clickable and page gets open successfully</t>
+  </si>
+  <si>
+    <t>Login and Logout</t>
+  </si>
+  <si>
+    <t>To check About Us link present and About Us page should get open successfully</t>
   </si>
 </sst>
 </file>
@@ -665,12 +701,291 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
+    <tabColor rgb="FF002060"/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="30">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -848,10 +1163,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="3" t="s">
         <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>33</v>
@@ -868,10 +1183,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>34</v>
@@ -888,10 +1203,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>35</v>
@@ -908,10 +1223,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>36</v>
@@ -928,10 +1243,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>37</v>
@@ -948,10 +1263,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>38</v>
@@ -968,10 +1283,10 @@
         <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>39</v>
@@ -984,10 +1299,10 @@
         <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>40</v>
@@ -995,22 +1310,22 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6" ht="45">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30">
@@ -1018,11 +1333,9 @@
         <v>30</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1033,7 +1346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -1041,7 +1354,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D7" sqref="D7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1112,7 +1425,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1132,7 +1445,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1152,7 +1465,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1170,7 +1483,7 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1184,11 +1497,11 @@
         <v>72</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1284,7 +1597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -1493,7 +1806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -1540,7 +1853,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
@@ -1558,7 +1871,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -1572,7 +1885,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -1586,7 +1899,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -1600,7 +1913,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -1614,7 +1927,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1626,7 +1939,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1638,7 +1951,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1650,7 +1963,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1702,7 +2015,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -1749,7 +2062,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
@@ -1767,7 +2080,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -1781,7 +2094,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -1795,7 +2108,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -1809,7 +2122,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -1823,7 +2136,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1835,7 +2148,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1847,7 +2160,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1859,7 +2172,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1911,7 +2224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1958,7 +2271,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
@@ -1976,7 +2289,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -1990,7 +2303,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -2004,7 +2317,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -2018,7 +2331,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -2032,7 +2345,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2044,7 +2357,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2056,7 +2369,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -2068,7 +2381,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -2120,7 +2433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -2167,7 +2480,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
@@ -2185,7 +2498,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -2199,7 +2512,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -2213,7 +2526,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -2227,7 +2540,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -2241,7 +2554,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2253,7 +2566,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2265,7 +2578,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -2277,7 +2590,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -2327,181 +2640,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <tabColor rgb="FF002060"/>
-  </sheetPr>
-  <dimension ref="A1:F14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>